<commit_message>
Update Stage Fright Project Plan.xlsx
</commit_message>
<xml_diff>
--- a/info/Stage Fright Project Plan.xlsx
+++ b/info/Stage Fright Project Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PS25JHill\Documents\tests\tests\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PS25JHill\Documents\Stage-Fright\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7F2979-572D-4674-B18B-2D2165AADCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA7E6B5-5F86-449D-B372-A4FFD0C67967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="5400" windowWidth="25710" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26760" yWindow="0" windowWidth="25905" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Task  Registration 11/1  Due 1/13</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Aidien and Jabari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aidien </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aidien sean </t>
+  </si>
+  <si>
+    <t>Aidien and Gabe</t>
   </si>
 </sst>
 </file>
@@ -324,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -354,6 +363,7 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +585,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -612,10 +622,14 @@
         <v>45604</v>
       </c>
       <c r="H1" s="4">
-        <v>45629</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
+        <v>45632</v>
+      </c>
+      <c r="I1" s="4">
+        <v>45639</v>
+      </c>
+      <c r="J1" s="5">
+        <v>45646</v>
+      </c>
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
@@ -642,8 +656,8 @@
       <c r="F3" s="20"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -658,8 +672,8 @@
       <c r="F4" s="19"/>
       <c r="G4" s="25"/>
       <c r="H4" s="26"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -674,8 +688,8 @@
       <c r="F5" s="10"/>
       <c r="G5" s="21"/>
       <c r="H5" s="25"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -690,8 +704,8 @@
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -706,8 +720,8 @@
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
       <c r="H7" s="26"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -722,8 +736,8 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="16"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -738,8 +752,8 @@
       <c r="F9" s="12"/>
       <c r="G9" s="10"/>
       <c r="H9" s="26"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -754,8 +768,8 @@
       <c r="F10" s="12"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="16"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -763,15 +777,15 @@
         <v>21</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -779,43 +793,47 @@
         <v>22</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="21"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="15"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="24"/>
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -971,11 +989,11 @@
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="17"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="27"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>